<commit_message>
Add basic button, text tield and background image for the purpose of testing
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="61">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -147,6 +147,57 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPOGRAPHY NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">UID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZCZYGIEŁ TO CHUJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPAŁA TO KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPAŁA TO KROL STM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
   </si>
 </sst>
 </file>
@@ -1369,6 +1420,9 @@
       <c r="I3" s="21" t="s">
         <v>36</v>
       </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -1387,6 +1441,7 @@
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
+      <c r="J4"/>
       <c r="K4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1420,6 +1475,7 @@
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1451,6 +1507,7 @@
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
+      <c r="J6"/>
       <c r="K6" s="8" t="s">
         <v>2</v>
       </c>
@@ -1596,33 +1653,56 @@
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
+      <c r="F3" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1"/>
-    <row r="5" spans="2:10" ht="15" customHeight="1"/>
+    <row r="4" spans="2:10" ht="15" customHeight="1">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="6" spans="2:10"/>
     <row r="7" spans="2:10"/>
     <row r="8" spans="2:10"/>

</xml_diff>

<commit_message>
Add some WIP changes for model - view - presenter
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="77">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t xml:space="preserve">OurTypography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essa</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1812,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:10"/>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="9" spans="2:10"/>
     <row r="10" spans="2:10"/>
     <row r="13" spans="2:10"/>

</xml_diff>

<commit_message>
Some code cleanup. Added invalidation for buttons and text fields in view class
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="78">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve">essa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Add more images for avatars. Add basis of write method in AuthScreenView
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="91">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -264,6 +264,37 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTER WITH THAT CARD
+YOU HOE FUCKING</t>
   </si>
 </sst>
 </file>
@@ -1915,7 +1946,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:10"/>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="14" spans="2:10"/>
     <row r="15" spans="2:10"/>
     <row r="16" spans="2:10"/>

</xml_diff>

<commit_message>
Add text field for showing which avatar has been saved
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3924" uniqueCount="104">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -304,6 +304,40 @@
   </si>
   <si>
     <t xml:space="preserve">Waiting for card...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVED: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZCZYGIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saved_resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT THE CARD 
+ON THE READER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT THE CARD 
+ON THE READER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT THE CARD 
+ON THE READER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT THE CARD 
+ON THE READER</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1577,9 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4"/>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
       <c r="G4"/>
       <c r="H4" t="s">
         <v>69</v>
@@ -1579,7 +1615,9 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5"/>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
       <c r="G5"/>
       <c r="H5" t="s">
         <v>69</v>
@@ -1613,7 +1651,9 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6"/>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
       <c r="G6"/>
       <c r="H6" t="s">
         <v>69</v>
@@ -1652,7 +1692,7 @@
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1966,7 +2006,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
@@ -1989,9 +2029,57 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:10"/>
-    <row r="16" spans="2:10"/>
-    <row r="17" spans="4:4"/>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="18" spans="4:4"/>
     <row r="19" spans="4:4"/>
     <row r="20" spans="4:4"/>

</xml_diff>

<commit_message>
Add sign out button in auth view
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3924" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4092" uniqueCount="106">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -338,6 +338,12 @@
   <si>
     <t xml:space="preserve">PUT THE CARD 
 ON THE READER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign out</t>
   </si>
 </sst>
 </file>
@@ -1861,16 +1867,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
@@ -1878,16 +1884,16 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
@@ -1895,16 +1901,16 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -1912,16 +1918,16 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
         <v>51</v>
@@ -1929,16 +1935,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -1946,7 +1952,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
@@ -1955,7 +1961,7 @@
         <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
         <v>51</v>
@@ -1963,16 +1969,16 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
@@ -1980,16 +1986,16 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
         <v>51</v>
@@ -1997,16 +2003,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
@@ -2014,72 +2020,24 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="B17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-    </row>
+    <row r="15" spans="2:10"/>
+    <row r="16" spans="2:10"/>
+    <row r="17" spans="4:4"/>
     <row r="18" spans="4:4"/>
     <row r="19" spans="4:4"/>
     <row r="20" spans="4:4"/>

</xml_diff>

<commit_message>
Add confirm choice button
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4092" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4616" uniqueCount="111">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -344,6 +344,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sign out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHOSEN: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1601,9 @@
       <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>110</v>
+      </c>
       <c r="H4" t="s">
         <v>69</v>
       </c>
@@ -1624,7 +1641,9 @@
       <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
       <c r="H5" t="s">
         <v>69</v>
       </c>
@@ -1660,7 +1679,9 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
       <c r="H6" t="s">
         <v>69</v>
       </c>
@@ -1696,7 +1717,9 @@
       <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="s">
+        <v>110</v>
+      </c>
       <c r="H7" t="s">
         <v>69</v>
       </c>
@@ -1989,13 +2012,13 @@
         <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="F12" t="s">
         <v>51</v>
@@ -2003,16 +2026,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
@@ -2020,7 +2043,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
@@ -2029,7 +2052,7 @@
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Some small changes. Attempt made to fix problem with images being handled wrong way
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4616" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4798" uniqueCount="113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t xml:space="preserve">:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You chose &lt;value&gt;. Waiting for the card to be applied... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You chose &lt;value&gt;. Waiting for card...</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1990,7 @@
         <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
         <v>51</v>

</xml_diff>